<commit_message>
Abstraction and MI  28-12-2023
</commit_message>
<xml_diff>
--- a/Updates.xlsx
+++ b/Updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java Full Stack\JAVA\CORE\OnlineTraining9\Sai\Java Fsd 12 th 2023 Dec\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC5292E-BBED-4BBE-965B-D2C427541059}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62905123-B391-45F2-8E84-ED6D000F9388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="58">
   <si>
     <t>Concepts</t>
   </si>
@@ -197,6 +197,9 @@
   </si>
   <si>
     <t>Inheritance and different levels abstract methods and concrete methods intro</t>
+  </si>
+  <si>
+    <t>Abstract class,interface,class,methods</t>
   </si>
 </sst>
 </file>
@@ -648,7 +651,7 @@
   <dimension ref="A3:M171"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14:G15"/>
+      <selection activeCell="G15" sqref="G15:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -880,9 +883,15 @@
       <c r="D16" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
+      <c r="E16" s="4">
+        <v>45288</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>

</xml_diff>